<commit_message>
Categorizzazione della feature 'Age' e ulteriore analisi dei dati
</commit_message>
<xml_diff>
--- a/dataset/Dataset.xlsx
+++ b/dataset/Dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\PycharmProjects\BDCM Blood Donor Classification Model\BDCM\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD68EB7-C25F-4F75-B1DF-499CA3E5E90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BD69C5-DF3E-421C-9328-A5D8C2988287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C6FBB159-9121-40E3-A0CF-0037408D1855}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3757" uniqueCount="1342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3774" uniqueCount="1354">
   <si>
     <t>Recency</t>
   </si>
@@ -4084,6 +4084,42 @@
   </si>
   <si>
     <t>Sinkkonen, Miss. Anna</t>
+  </si>
+  <si>
+    <t>28.5</t>
+  </si>
+  <si>
+    <t>70.5</t>
+  </si>
+  <si>
+    <t>32.5</t>
+  </si>
+  <si>
+    <t>36.5</t>
+  </si>
+  <si>
+    <t>55.5</t>
+  </si>
+  <si>
+    <t>40.5</t>
+  </si>
+  <si>
+    <t>45.5</t>
+  </si>
+  <si>
+    <t>20.5</t>
+  </si>
+  <si>
+    <t>23.5</t>
+  </si>
+  <si>
+    <t>24.5</t>
+  </si>
+  <si>
+    <t>22.5</t>
+  </si>
+  <si>
+    <t>37.5</t>
   </si>
 </sst>
 </file>
@@ -4163,12 +4199,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -4569,8 +4608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF776D7-8329-4281-BBAC-1920689CA610}">
   <dimension ref="A1:H749"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A723" workbookViewId="0">
-      <selection activeCell="G746" sqref="G746"/>
+    <sheetView tabSelected="1" topLeftCell="A696" workbookViewId="0">
+      <selection activeCell="D697" sqref="D697"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4615,7 +4654,7 @@
       <c r="B2" t="s">
         <v>757</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>22</v>
       </c>
       <c r="D2">
@@ -4641,7 +4680,7 @@
       <c r="B3" t="s">
         <v>760</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>38</v>
       </c>
       <c r="D3">
@@ -4792,7 +4831,7 @@
         <v>757</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -4844,7 +4883,7 @@
         <v>760</v>
       </c>
       <c r="C11">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -4870,7 +4909,7 @@
         <v>760</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -4974,7 +5013,7 @@
         <v>760</v>
       </c>
       <c r="C16">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -5023,7 +5062,7 @@
         <v>757</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -5170,7 +5209,7 @@
         <v>760</v>
       </c>
       <c r="C24">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="D24">
         <v>2</v>
@@ -5222,7 +5261,7 @@
         <v>760</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D26">
         <v>9</v>
@@ -5594,7 +5633,7 @@
         <v>760</v>
       </c>
       <c r="C41">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="D41">
         <v>4</v>
@@ -5695,7 +5734,7 @@
         <v>760</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D45">
         <v>2</v>
@@ -5865,7 +5904,7 @@
         <v>757</v>
       </c>
       <c r="C52">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="D52">
         <v>2</v>
@@ -6043,8 +6082,8 @@
       <c r="B59" t="s">
         <v>757</v>
       </c>
-      <c r="C59">
-        <v>285</v>
+      <c r="C59" s="5" t="s">
+        <v>1342</v>
       </c>
       <c r="D59">
         <v>2</v>
@@ -6070,7 +6109,7 @@
         <v>760</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="D60">
         <v>2</v>
@@ -6096,7 +6135,7 @@
         <v>757</v>
       </c>
       <c r="C61">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D61">
         <v>3</v>
@@ -6197,7 +6236,7 @@
         <v>757</v>
       </c>
       <c r="C65">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="D65">
         <v>4</v>
@@ -6321,7 +6360,7 @@
         <v>760</v>
       </c>
       <c r="C70">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D70">
         <v>4</v>
@@ -6399,7 +6438,7 @@
         <v>760</v>
       </c>
       <c r="C73">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D73">
         <v>2</v>
@@ -6728,7 +6767,7 @@
         <v>760</v>
       </c>
       <c r="C86">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D86">
         <v>2</v>
@@ -6780,7 +6819,7 @@
         <v>757</v>
       </c>
       <c r="C88">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D88">
         <v>4</v>
@@ -7414,8 +7453,8 @@
       <c r="B113" t="s">
         <v>760</v>
       </c>
-      <c r="C113">
-        <v>145</v>
+      <c r="C113" s="5" t="s">
+        <v>1351</v>
       </c>
       <c r="D113">
         <v>4</v>
@@ -7493,7 +7532,7 @@
         <v>760</v>
       </c>
       <c r="C116">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D116">
         <v>2</v>
@@ -7544,8 +7583,8 @@
       <c r="B118" t="s">
         <v>757</v>
       </c>
-      <c r="C118">
-        <v>705</v>
+      <c r="C118" s="5" t="s">
+        <v>1343</v>
       </c>
       <c r="D118">
         <v>2</v>
@@ -7623,7 +7662,7 @@
         <v>760</v>
       </c>
       <c r="C121">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D121">
         <v>2</v>
@@ -7697,8 +7736,8 @@
       <c r="B124" t="s">
         <v>757</v>
       </c>
-      <c r="C124">
-        <v>325</v>
+      <c r="C124" s="5" t="s">
+        <v>1344</v>
       </c>
       <c r="D124">
         <v>2</v>
@@ -7723,8 +7762,8 @@
       <c r="B125" t="s">
         <v>760</v>
       </c>
-      <c r="C125">
-        <v>325</v>
+      <c r="C125" s="5" t="s">
+        <v>1344</v>
       </c>
       <c r="D125">
         <v>2</v>
@@ -7776,7 +7815,7 @@
         <v>757</v>
       </c>
       <c r="C127">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D127">
         <v>2</v>
@@ -8102,7 +8141,7 @@
         <v>757</v>
       </c>
       <c r="C140">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D140">
         <v>9</v>
@@ -8333,7 +8372,7 @@
         <v>760</v>
       </c>
       <c r="C149">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D149">
         <v>2</v>
@@ -8358,8 +8397,8 @@
       <c r="B150" t="s">
         <v>757</v>
       </c>
-      <c r="C150">
-        <v>365</v>
+      <c r="C150" s="5" t="s">
+        <v>1345</v>
       </c>
       <c r="D150">
         <v>2</v>
@@ -8462,8 +8501,8 @@
       <c r="B154" t="s">
         <v>757</v>
       </c>
-      <c r="C154">
-        <v>555</v>
+      <c r="C154" s="5" t="s">
+        <v>1346</v>
       </c>
       <c r="D154">
         <v>4</v>
@@ -8488,8 +8527,8 @@
       <c r="B155" t="s">
         <v>757</v>
       </c>
-      <c r="C155">
-        <v>405</v>
+      <c r="C155" s="5" t="s">
+        <v>1347</v>
       </c>
       <c r="D155">
         <v>2</v>
@@ -8563,8 +8602,8 @@
       <c r="B158" t="s">
         <v>760</v>
       </c>
-      <c r="C158">
-        <v>16</v>
+      <c r="C158" s="5" t="s">
+        <v>1353</v>
       </c>
       <c r="D158">
         <v>2</v>
@@ -8740,7 +8779,7 @@
         <v>757</v>
       </c>
       <c r="C165">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D165">
         <v>2</v>
@@ -8766,7 +8805,7 @@
         <v>757</v>
       </c>
       <c r="C166">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D166">
         <v>2</v>
@@ -8792,7 +8831,7 @@
         <v>757</v>
       </c>
       <c r="C167">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="D167">
         <v>2</v>
@@ -8942,7 +8981,7 @@
         <v>757</v>
       </c>
       <c r="C173">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="D173">
         <v>2</v>
@@ -8968,7 +9007,7 @@
         <v>760</v>
       </c>
       <c r="C174">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D174">
         <v>2</v>
@@ -9219,7 +9258,7 @@
         <v>757</v>
       </c>
       <c r="C184">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D184">
         <v>2</v>
@@ -9245,7 +9284,7 @@
         <v>757</v>
       </c>
       <c r="C185">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="D185">
         <v>4</v>
@@ -9271,7 +9310,7 @@
         <v>760</v>
       </c>
       <c r="C186">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="D186">
         <v>13</v>
@@ -9499,7 +9538,7 @@
         <v>757</v>
       </c>
       <c r="C195">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="D195">
         <v>11</v>
@@ -9749,8 +9788,8 @@
       <c r="B205" t="s">
         <v>757</v>
       </c>
-      <c r="C205">
-        <v>455</v>
+      <c r="C205" s="5" t="s">
+        <v>1348</v>
       </c>
       <c r="D205">
         <v>4</v>
@@ -9802,7 +9841,7 @@
         <v>760</v>
       </c>
       <c r="C207">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="D207">
         <v>11</v>
@@ -9880,7 +9919,7 @@
         <v>760</v>
       </c>
       <c r="C210">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D210">
         <v>11</v>
@@ -10189,7 +10228,7 @@
         <v>757</v>
       </c>
       <c r="C222">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D222">
         <v>4</v>
@@ -10367,8 +10406,8 @@
       <c r="B229" t="s">
         <v>757</v>
       </c>
-      <c r="C229">
-        <v>205</v>
+      <c r="C229" s="5" t="s">
+        <v>1349</v>
       </c>
       <c r="D229">
         <v>4</v>
@@ -10521,7 +10560,7 @@
         <v>760</v>
       </c>
       <c r="C235">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="D235">
         <v>10</v>
@@ -10622,7 +10661,7 @@
         <v>760</v>
       </c>
       <c r="C239">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D239">
         <v>4</v>
@@ -11228,7 +11267,7 @@
         <v>757</v>
       </c>
       <c r="C263">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="D263">
         <v>11</v>
@@ -11355,7 +11394,7 @@
         <v>757</v>
       </c>
       <c r="C268">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D268">
         <v>3</v>
@@ -11658,7 +11697,7 @@
         <v>757</v>
       </c>
       <c r="C280">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="D280">
         <v>14</v>
@@ -11762,7 +11801,7 @@
         <v>757</v>
       </c>
       <c r="C284">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D284">
         <v>14</v>
@@ -12119,8 +12158,8 @@
       <c r="B298" t="s">
         <v>757</v>
       </c>
-      <c r="C298">
-        <v>235</v>
+      <c r="C298" s="5" t="s">
+        <v>1350</v>
       </c>
       <c r="D298">
         <v>14</v>
@@ -12146,7 +12185,7 @@
         <v>760</v>
       </c>
       <c r="C299">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D299">
         <v>14</v>
@@ -12385,7 +12424,7 @@
         <v>760</v>
       </c>
       <c r="C309">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D309">
         <v>11</v>
@@ -12954,7 +12993,7 @@
         <v>760</v>
       </c>
       <c r="C331">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D331">
         <v>16</v>
@@ -13002,8 +13041,8 @@
       <c r="B333" t="s">
         <v>757</v>
       </c>
-      <c r="C333">
-        <v>455</v>
+      <c r="C333" s="5" t="s">
+        <v>1348</v>
       </c>
       <c r="D333">
         <v>16</v>
@@ -13055,7 +13094,7 @@
         <v>757</v>
       </c>
       <c r="C335">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D335">
         <v>11</v>
@@ -13231,7 +13270,7 @@
         <v>757</v>
       </c>
       <c r="C342">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D342">
         <v>14</v>
@@ -13436,7 +13475,7 @@
         <v>757</v>
       </c>
       <c r="C350">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D350">
         <v>11</v>
@@ -13537,7 +13576,7 @@
         <v>757</v>
       </c>
       <c r="C354">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D354">
         <v>11</v>
@@ -14091,7 +14130,7 @@
         <v>760</v>
       </c>
       <c r="C376">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="D376">
         <v>14</v>
@@ -14270,7 +14309,7 @@
         <v>760</v>
       </c>
       <c r="C383">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D383">
         <v>14</v>
@@ -14397,7 +14436,7 @@
         <v>757</v>
       </c>
       <c r="C388">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="D388">
         <v>14</v>
@@ -14472,7 +14511,7 @@
         <v>760</v>
       </c>
       <c r="C391">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="D391">
         <v>14</v>
@@ -14940,7 +14979,7 @@
         <v>757</v>
       </c>
       <c r="C409">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="D409">
         <v>16</v>
@@ -15237,7 +15276,7 @@
         <v>760</v>
       </c>
       <c r="C421">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D421">
         <v>16</v>
@@ -15589,7 +15628,7 @@
         <v>757</v>
       </c>
       <c r="C435">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D435">
         <v>14</v>
@@ -15641,7 +15680,7 @@
         <v>760</v>
       </c>
       <c r="C437">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="D437">
         <v>16</v>
@@ -15898,7 +15937,7 @@
         <v>757</v>
       </c>
       <c r="C447">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D447">
         <v>21</v>
@@ -15924,7 +15963,7 @@
         <v>760</v>
       </c>
       <c r="C448">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D448">
         <v>23</v>
@@ -15976,7 +16015,7 @@
         <v>760</v>
       </c>
       <c r="C450">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="D450">
         <v>23</v>
@@ -16755,7 +16794,7 @@
         <v>760</v>
       </c>
       <c r="C481">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="D481">
         <v>23</v>
@@ -16781,7 +16820,7 @@
         <v>757</v>
       </c>
       <c r="C482">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="D482">
         <v>23</v>
@@ -17009,7 +17048,7 @@
         <v>757</v>
       </c>
       <c r="C491">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D491">
         <v>21</v>
@@ -17286,7 +17325,7 @@
         <v>757</v>
       </c>
       <c r="C502">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D502">
         <v>2</v>
@@ -17387,7 +17426,7 @@
         <v>760</v>
       </c>
       <c r="C506">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="D506">
         <v>0</v>
@@ -17917,8 +17956,8 @@
       <c r="B527" t="s">
         <v>757</v>
       </c>
-      <c r="C527">
-        <v>405</v>
+      <c r="C527" s="5" t="s">
+        <v>1347</v>
       </c>
       <c r="D527">
         <v>2</v>
@@ -18045,7 +18084,7 @@
         <v>760</v>
       </c>
       <c r="C532">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D532">
         <v>4</v>
@@ -18094,7 +18133,7 @@
         <v>757</v>
       </c>
       <c r="C534">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D534">
         <v>4</v>
@@ -18169,7 +18208,7 @@
         <v>760</v>
       </c>
       <c r="C537">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="D537">
         <v>4</v>
@@ -18322,7 +18361,7 @@
         <v>760</v>
       </c>
       <c r="C543">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D543">
         <v>2</v>
@@ -18348,7 +18387,7 @@
         <v>760</v>
       </c>
       <c r="C544">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D544">
         <v>4</v>
@@ -18527,7 +18566,7 @@
         <v>757</v>
       </c>
       <c r="C551">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D551">
         <v>4</v>
@@ -18553,7 +18592,7 @@
         <v>757</v>
       </c>
       <c r="C552">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D552">
         <v>4</v>
@@ -19156,7 +19195,7 @@
         <v>757</v>
       </c>
       <c r="C576">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D576">
         <v>2</v>
@@ -20267,7 +20306,7 @@
         <v>760</v>
       </c>
       <c r="C620">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="D620">
         <v>4</v>
@@ -20677,7 +20716,7 @@
         <v>760</v>
       </c>
       <c r="C636">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="D636">
         <v>13</v>
@@ -20879,7 +20918,7 @@
         <v>760</v>
       </c>
       <c r="C644">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D644">
         <v>11</v>
@@ -21738,8 +21777,8 @@
       <c r="B678" t="s">
         <v>757</v>
       </c>
-      <c r="C678">
-        <v>245</v>
+      <c r="C678" s="5" t="s">
+        <v>1351</v>
       </c>
       <c r="D678">
         <v>14</v>
@@ -21918,7 +21957,7 @@
         <v>757</v>
       </c>
       <c r="C685">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D685">
         <v>11</v>
@@ -21996,7 +22035,7 @@
         <v>757</v>
       </c>
       <c r="C688">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="D688">
         <v>13</v>
@@ -22073,8 +22112,8 @@
       <c r="B691" t="s">
         <v>760</v>
       </c>
-      <c r="C691">
-        <v>15</v>
+      <c r="C691" s="5" t="s">
+        <v>1352</v>
       </c>
       <c r="D691">
         <v>14</v>
@@ -22126,7 +22165,7 @@
         <v>760</v>
       </c>
       <c r="C693">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="D693">
         <v>14</v>
@@ -22865,7 +22904,7 @@
         <v>760</v>
       </c>
       <c r="C722">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D722">
         <v>21</v>
@@ -22891,7 +22930,7 @@
         <v>757</v>
       </c>
       <c r="C723">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D723">
         <v>23</v>
@@ -23145,7 +23184,7 @@
         <v>757</v>
       </c>
       <c r="C733">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="D733">
         <v>14</v>
@@ -23245,8 +23284,8 @@
       <c r="B737" t="s">
         <v>757</v>
       </c>
-      <c r="C737">
-        <v>285</v>
+      <c r="C737" s="5" t="s">
+        <v>1342</v>
       </c>
       <c r="D737">
         <v>23</v>
@@ -23523,7 +23562,7 @@
         <v>757</v>
       </c>
       <c r="C748">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D748">
         <v>39</v>
@@ -23579,7 +23618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF38908A-7005-492C-B7C1-75C5F0E61443}">
   <dimension ref="A1:I749"/>
   <sheetViews>
-    <sheetView topLeftCell="A739" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H749" sqref="H749"/>
     </sheetView>
   </sheetViews>

</xml_diff>